<commit_message>
Merge remote-racking branch 'origin/Nikita' into Nikita
</commit_message>
<xml_diff>
--- a/data/2021-11-19 Roder связи.xlsx
+++ b/data/2021-11-19 Roder связи.xlsx
@@ -1229,11 +1229,11 @@
   </sheetPr>
   <dimension ref="A1:N116"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.48828125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.45"/>
@@ -1243,10 +1243,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="230.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="73.85"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1290,7 +1291,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>14</v>
       </c>
@@ -1307,7 +1308,7 @@
         <v>44578</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>16</v>
       </c>
@@ -1324,7 +1325,7 @@
         <v>44578</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>18</v>
       </c>
@@ -1344,7 +1345,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" s="4" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -1368,7 +1369,7 @@
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>25</v>
       </c>
@@ -1388,7 +1389,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" s="4" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
@@ -1412,7 +1413,7 @@
       </c>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" s="4" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
@@ -1436,7 +1437,7 @@
       </c>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" s="4" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
@@ -1460,7 +1461,7 @@
       </c>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" s="4" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
@@ -1484,7 +1485,7 @@
       </c>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" s="4" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>40</v>
       </c>
@@ -1508,7 +1509,7 @@
       </c>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>43</v>
       </c>
@@ -1525,7 +1526,7 @@
         <v>44524</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>44</v>
       </c>
@@ -1542,7 +1543,7 @@
         <v>44496</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>45</v>
       </c>
@@ -1568,7 +1569,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>50</v>
       </c>
@@ -1585,7 +1586,7 @@
         <v>44524</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>51</v>
       </c>
@@ -1611,7 +1612,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>55</v>
       </c>
@@ -1628,7 +1629,7 @@
         <v>44503</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>56</v>
       </c>
@@ -1657,7 +1658,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>60</v>
       </c>
@@ -1686,7 +1687,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>63</v>
       </c>
@@ -1715,7 +1716,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>66</v>
       </c>
@@ -1744,7 +1745,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>69</v>
       </c>
@@ -1773,7 +1774,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>72</v>
       </c>
@@ -1802,7 +1803,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>75</v>
       </c>
@@ -1831,7 +1832,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>78</v>
       </c>
@@ -1863,7 +1864,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>81</v>
       </c>
@@ -1880,7 +1881,7 @@
         <v>44573</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>82</v>
       </c>
@@ -1897,7 +1898,7 @@
         <v>44568</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>83</v>
       </c>
@@ -1914,7 +1915,7 @@
         <v>44531</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>85</v>
       </c>
@@ -1949,7 +1950,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>91</v>
       </c>
@@ -1966,7 +1967,7 @@
         <v>44561</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>93</v>
       </c>
@@ -2001,7 +2002,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>99</v>
       </c>
@@ -2036,7 +2037,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>102</v>
       </c>
@@ -2071,7 +2072,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>104</v>
       </c>
@@ -2106,7 +2107,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>108</v>
       </c>
@@ -2141,7 +2142,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>110</v>
       </c>
@@ -2164,7 +2165,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>114</v>
       </c>
@@ -2199,7 +2200,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>119</v>
       </c>
@@ -2234,7 +2235,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>122</v>
       </c>
@@ -2269,7 +2270,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>125</v>
       </c>
@@ -2304,7 +2305,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>127</v>
       </c>
@@ -2321,7 +2322,7 @@
         <v>44547</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>129</v>
       </c>
@@ -2356,7 +2357,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>135</v>
       </c>
@@ -2388,7 +2389,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>140</v>
       </c>
@@ -2420,7 +2421,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>144</v>
       </c>
@@ -2437,7 +2438,7 @@
         <v>44550</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>146</v>
       </c>
@@ -2472,7 +2473,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>150</v>
       </c>
@@ -2489,7 +2490,7 @@
         <v>44564</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>152</v>
       </c>
@@ -2527,7 +2528,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>158</v>
       </c>
@@ -2562,7 +2563,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>161</v>
       </c>
@@ -2600,7 +2601,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>164</v>
       </c>
@@ -2635,7 +2636,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>169</v>
       </c>
@@ -2652,7 +2653,7 @@
         <v>44568</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>170</v>
       </c>
@@ -2690,7 +2691,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>174</v>
       </c>
@@ -2725,7 +2726,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>176</v>
       </c>
@@ -2742,7 +2743,7 @@
         <v>44573</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>177</v>
       </c>
@@ -2774,7 +2775,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>183</v>
       </c>
@@ -2806,7 +2807,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>186</v>
       </c>
@@ -2838,7 +2839,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>188</v>
       </c>
@@ -2870,7 +2871,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>193</v>
       </c>
@@ -2902,7 +2903,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>195</v>
       </c>
@@ -2934,7 +2935,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>197</v>
       </c>
@@ -2966,7 +2967,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>199</v>
       </c>
@@ -2998,7 +2999,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>202</v>
       </c>
@@ -3015,7 +3016,7 @@
         <v>44573</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>203</v>
       </c>
@@ -3032,7 +3033,7 @@
         <v>44573</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>204</v>
       </c>
@@ -3064,7 +3065,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>209</v>
       </c>
@@ -3096,7 +3097,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>211</v>
       </c>
@@ -3113,7 +3114,7 @@
         <v>44573</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>212</v>
       </c>
@@ -3145,7 +3146,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>215</v>
       </c>
@@ -3177,7 +3178,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>217</v>
       </c>
@@ -3194,7 +3195,7 @@
         <v>44573</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>218</v>
       </c>
@@ -3226,7 +3227,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>221</v>
       </c>
@@ -3258,7 +3259,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>223</v>
       </c>
@@ -3290,7 +3291,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>225</v>
       </c>
@@ -3307,7 +3308,7 @@
         <v>44573</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>226</v>
       </c>
@@ -3324,7 +3325,7 @@
         <v>44573</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>227</v>
       </c>
@@ -3356,7 +3357,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>232</v>
       </c>
@@ -3388,7 +3389,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>235</v>
       </c>
@@ -3420,7 +3421,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>237</v>
       </c>
@@ -3452,7 +3453,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>239</v>
       </c>
@@ -3484,7 +3485,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>242</v>
       </c>
@@ -3516,7 +3517,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>244</v>
       </c>
@@ -3548,7 +3549,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>247</v>
       </c>
@@ -3565,7 +3566,7 @@
         <v>44573</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>248</v>
       </c>
@@ -3597,7 +3598,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>253</v>
       </c>
@@ -3629,7 +3630,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>256</v>
       </c>
@@ -3661,7 +3662,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>258</v>
       </c>
@@ -3693,7 +3694,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>261</v>
       </c>
@@ -3725,7 +3726,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>263</v>
       </c>
@@ -3757,7 +3758,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>265</v>
       </c>
@@ -3774,7 +3775,7 @@
         <v>44572</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>266</v>
       </c>
@@ -3806,7 +3807,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>271</v>
       </c>
@@ -3838,7 +3839,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>274</v>
       </c>
@@ -3870,7 +3871,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>277</v>
       </c>
@@ -3887,7 +3888,7 @@
         <v>44567</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>278</v>
       </c>
@@ -3919,7 +3920,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>283</v>
       </c>
@@ -3951,7 +3952,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
         <v>285</v>
       </c>
@@ -3968,7 +3969,7 @@
         <v>44572</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>286</v>
       </c>
@@ -4000,7 +4001,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>291</v>
       </c>
@@ -4032,7 +4033,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>295</v>
       </c>
@@ -4064,7 +4065,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>299</v>
       </c>
@@ -4081,7 +4082,7 @@
         <v>44567</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>300</v>
       </c>
@@ -4113,7 +4114,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
         <v>305</v>
       </c>
@@ -4145,7 +4146,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>309</v>
       </c>
@@ -4177,7 +4178,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>313</v>
       </c>
@@ -4209,7 +4210,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>317</v>
       </c>
@@ -4226,7 +4227,7 @@
         <v>44578</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
         <v>318</v>
       </c>
@@ -4243,7 +4244,7 @@
         <v>44578</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>319</v>
       </c>
@@ -4275,7 +4276,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>322</v>
       </c>
@@ -4307,7 +4308,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
         <v>324</v>
       </c>
@@ -4339,7 +4340,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>326</v>
       </c>
@@ -4371,7 +4372,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>328</v>
       </c>
@@ -4403,7 +4404,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
         <v>330</v>
       </c>
@@ -4435,7 +4436,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
         <v>332</v>
       </c>
@@ -4467,7 +4468,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
         <v>334</v>
       </c>
@@ -4508,254 +4509,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Документ" ma:contentTypeID="0x010100CE6AFE74FDD415468BC9C30152D840F6" ma:contentTypeVersion="13" ma:contentTypeDescription="Создание документа." ma:contentTypeScope="" ma:versionID="3aff26cacd26e777a7c9e11a88147115">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="42664ea3-8066-40f9-a3a7-1ee510d0e58e" xmlns:ns3="401ce9f9-7438-4061-9620-45eeac52959f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="26a7652d10a6617a2141ce34bf6d1c49" ns2:_="" ns3:_="">
-    <xsd:import namespace="42664ea3-8066-40f9-a3a7-1ee510d0e58e"/>
-    <xsd:import namespace="401ce9f9-7438-4061-9620-45eeac52959f"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="42664ea3-8066-40f9-a3a7-1ee510d0e58e" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="11" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="12" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="13" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="15" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="18" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="19" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="401ce9f9-7438-4061-9620-45eeac52959f" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="16" nillable="true" ma:displayName="Общий доступ с использованием" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="17" nillable="true" ma:displayName="Совместно с подробностями" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Тип контента"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Название"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6AC60AB-E0F4-4ABC-BE7A-DA18EEDA2B55}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14581951-92EE-42F6-B913-F1D0D79ADB2C}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DB3852D-7194-415A-A457-71EA10EC7024}"/>
 </file>
</xml_diff>